<commit_message>
SE-391 Incorporated Bernd's changes that validate strains against the straindb
SVN: 23923
</commit_message>
<xml_diff>
--- a/eu_basynthec/sourceTest/examples/Transcriptomics-Example.xlsx
+++ b/eu_basynthec/sourceTest/examples/Transcriptomics-Example.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21105"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
@@ -73,14 +73,6 @@
     <t>tmk</t>
   </si>
   <si>
-    <t>MGP253-1 66687802</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MGP776-2 66730002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>One of CE, ES, ME, CY, or NC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -321,6 +313,12 @@
   </si>
   <si>
     <t>JJS-MGP776</t>
+  </si>
+  <si>
+    <t>JJS-MGP253-1 66687802</t>
+  </si>
+  <si>
+    <t>JJS-MGP776-2 66730002</t>
   </si>
 </sst>
 </file>
@@ -780,112 +778,112 @@
   <sheetData>
     <row r="1" spans="1:3" ht="20">
       <c r="A1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="9">
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -907,7 +905,7 @@
   <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -922,20 +920,20 @@
     <row r="1" spans="1:5">
       <c r="A1" s="11"/>
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="11"/>
       <c r="B2" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="11"/>
       <c r="D2" s="11">
@@ -948,7 +946,7 @@
     <row r="3" spans="1:5">
       <c r="A3" s="11"/>
       <c r="B3" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11">
@@ -961,7 +959,7 @@
     <row r="4" spans="1:5">
       <c r="A4" s="11"/>
       <c r="B4" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11">
@@ -973,27 +971,27 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>54</v>
-      </c>
       <c r="D5" s="12" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="12">
         <v>58</v>
@@ -1007,10 +1005,10 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C7" s="12">
         <v>49</v>
@@ -1024,10 +1022,10 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C8" s="12">
         <v>7</v>
@@ -1041,10 +1039,10 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C9" s="12">
         <v>48</v>
@@ -1058,10 +1056,10 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C10" s="12">
         <v>8</v>
@@ -1075,10 +1073,10 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C11" s="12">
         <v>84</v>
@@ -1092,10 +1090,10 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C12" s="12">
         <v>110</v>
@@ -1109,10 +1107,10 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C13" s="12">
         <v>64</v>
@@ -1126,10 +1124,10 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="12">
         <v>59</v>
@@ -1143,10 +1141,10 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="12">
         <v>38</v>
@@ -1160,10 +1158,10 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C16" s="12">
         <v>24</v>
@@ -1177,10 +1175,10 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="12">
         <v>8</v>
@@ -1194,10 +1192,10 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="14" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C18" s="12">
         <v>55</v>
@@ -1211,10 +1209,10 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C19" s="12">
         <v>19</v>
@@ -1228,10 +1226,10 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C20" s="12">
         <v>3</v>
@@ -1245,10 +1243,10 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C21" s="12">
         <v>74</v>
@@ -1262,7 +1260,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>0</v>

</xml_diff>